<commit_message>
100 percent validated, get_permits.py
</commit_message>
<xml_diff>
--- a/data/city_permits/raw/city_2015.xlsx
+++ b/data/city_permits/raw/city_2015.xlsx
@@ -257,14 +257,14 @@
         </is>
       </c>
       <c s="2" r="H1">
-        <v>42626</v>
+        <v>42628</v>
       </c>
     </row>
     <row r="2" ht="1" customHeight="1"/>
     <row r="3" ht="18" customHeight="1">
       <c s="1" t="inlineStr" r="A3">
         <is>
-          <t xml:space="preserve">For Permits Issued 1/1/2015 through 12/31/2015</t>
+          <t xml:space="preserve">For Permits Issued 01/01/2015 through 12/31/2015</t>
         </is>
       </c>
     </row>

</xml_diff>